<commit_message>
Dummies, SARIMA fix, LASSO and SARIMA re-run
</commit_message>
<xml_diff>
--- a/Data/data_NSA/Varmonth.xlsx
+++ b/Data/data_NSA/Varmonth.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad5e0ae908eb1af8/Documentos/GitHub/gdp-forecasting-with-ML/Data/data_NSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_AD4D361C20488DEA4E38A0E30418638E5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C7FD17D-AD9C-4C82-A11B-E514CC106353}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="11_AD4D361C20488DEA4E38A0E30418638E5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDC03B5E-40F4-4A53-A604-738FB4DEA417}"/>
   <bookViews>
     <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,8 +132,2541 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Plan1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ibc_rs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$A$2:$A$286</c:f>
+              <c:numCache>
+                <c:formatCode>yyyy\-mm\-dd</c:formatCode>
+                <c:ptCount val="285"/>
+                <c:pt idx="0">
+                  <c:v>37257</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37288</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37347</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37377</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37408</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37438</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37469</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>37530</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37561</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37591</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>37622</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>37653</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37681</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>37712</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>37742</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>37773</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37803</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37834</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>37865</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>37895</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>37926</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37956</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>37987</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>38018</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>38047</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38078</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38108</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>38139</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>38169</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>38200</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>38231</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38261</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38292</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>38322</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>38353</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38384</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38412</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>38443</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>38473</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>38504</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>38534</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>38565</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>38596</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>38626</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>38657</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>38687</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>38718</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>38749</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>38777</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>38808</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>38838</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>38869</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>38899</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>38930</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>38961</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>38991</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>39022</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>39052</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>39083</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>39114</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>39142</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>39173</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>39203</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>39234</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>39264</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>39295</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>39326</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>39356</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>39387</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>39417</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>39448</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>39479</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>39508</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>39539</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>39569</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>39600</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>39630</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>39661</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>39692</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>39722</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>39753</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>39783</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>39814</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>39845</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>39873</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>39904</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>39934</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>39965</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>39995</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>40026</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>40057</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>40087</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>40118</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>40148</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>40179</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>40210</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>40238</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>40269</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>40299</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>40330</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>40360</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>40391</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>40422</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>40452</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>40483</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>40513</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>40544</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>40575</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>40603</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>40634</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>40664</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>40695</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>40725</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>40756</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>40787</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>40817</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>40848</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>40878</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>40909</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>40940</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>41000</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>41030</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>41061</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>41091</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>41122</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>41153</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>41183</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>41214</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>41244</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>41275</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>41306</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>41334</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>41365</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>41395</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>41426</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>41456</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>41487</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>41518</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>41548</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>41579</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>41609</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>41640</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>41671</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>41699</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>41730</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>41760</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>41791</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>41821</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>41852</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>41883</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>41913</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>41944</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>41974</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>42005</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>42036</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>42064</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>42095</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>42125</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>42156</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>42186</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>42217</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>42248</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>42278</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>42309</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>42339</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>42370</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>42401</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>42430</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>42461</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>42491</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>42552</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>42583</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>42614</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>42644</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>42675</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>42705</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>42736</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>42767</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>42795</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>42826</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>42856</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>42917</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>42948</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>42979</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>43009</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>43040</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>43070</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>43252</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>43282</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>43313</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>43344</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>43374</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>43405</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>43435</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>43466</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>43497</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>43525</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>43556</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>43617</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>43647</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>43678</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>43709</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>43739</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>43770</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>43800</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>43831</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>43891</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>44075</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>44105</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>44136</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>44166</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>44409</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>44440</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>44470</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>44531</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>44593</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>44621</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>44652</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>44682</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>44713</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>44743</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>44774</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>44805</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>44835</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>44866</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>44896</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>44927</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>44958</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>44986</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>45017</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>45047</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>45078</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>45108</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>45139</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>45170</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>45200</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>45231</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>45261</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>45292</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>45323</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>45352</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>45383</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>45413</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>45444</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>45474</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>45505</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>45536</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>45566</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>45597</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>45627</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>45658</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>45689</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>45717</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>45748</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>45778</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>45809</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>45839</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>45870</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>45901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$B$2:$B$286</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="285"/>
+                <c:pt idx="12">
+                  <c:v>75.67</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>83.03</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96.55</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>88.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>75.45</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>69.45</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>69.05</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>67.91</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>69.010000000000005</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>73.62</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>75.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>74.81</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>76.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>80.739999999999995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>102.15</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>89.09</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>75.84</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>73.33</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>74.53</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>72.19</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>74.81</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>76.55</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>79.36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>75.42</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>77.11</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>93.48</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>84.16</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>76.39</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>74.78</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>74.02</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>74.540000000000006</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>70.53</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>73.14</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>75.77</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>78.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>77.959999999999994</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>80.89</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>94.71</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>85.29</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>80.209999999999994</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>76.239999999999995</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>76.680000000000007</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>77.349999999999994</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>75.17</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>77.819999999999993</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>78.569999999999993</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>81.510000000000005</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>82.77</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>86.15</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>100.37</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>92.56</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>85.41</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>80.510000000000005</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>81.48</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>81.83</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>78.150000000000006</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>83.92</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>85.14</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>86.69</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>86.15</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>90.27</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>101.66</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>96.89</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>87.03</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>85.4</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>85.96</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>84.23</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>84.7</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>84.54</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>84.97</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>83.55</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>87.82</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>106.68</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>97.89</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>86.15</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>84.45</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>85.13</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>83.95</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>83.72</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>87.32</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>87.37</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>92.29</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>88.64</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>92.99</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>114.18</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>103.92</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>91.13</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>89.52</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>91.01</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>89.52</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>86.68</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>89.39</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>94.03</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>95.58</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>93.7</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>99.98</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>118.93</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>107.54</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>96.39</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>92.96</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>93.36</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>94.07</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>91.52</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>94.34</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>97.1</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>100.02</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>94.06</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>95.62</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>109.26</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>100.55</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>97.07</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>93.85</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>94.76</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>97.71</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>91.53</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>97.33</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>98.28</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>97.26</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>98.71</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>103.78</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>120.35</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>115.97</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>101.27</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>97.41</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>101.24</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>101.37</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>97.75</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>103.99</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>103.92</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>100.8</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>102.35</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>109.42</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>126.27</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>116.73</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>101.18</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>93.76</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>97.45</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>97.67</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>97.8</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>101.41</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>100.54</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>101.2</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>99.25</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>105.28</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>128.68</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>115.76</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>92.03</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>94.56</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>92.71</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>90.57</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>93.39</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>92.87</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>94.75</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>93.2</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>101.43</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>119.27</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>109.1</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>93.73</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>91.52</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>90.17</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>92.27</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>91.34</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>92.77</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>93.27</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>94.86</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>105.28</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>127.27</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>111.49</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>96.33</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>91.81</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>91.82</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>92.68</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>89.03</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>91.72</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>93.63</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>96.92</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>96.08</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>102.27</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>120.5</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>112.05</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>93.26</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>94.28</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>95.84</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>98.32</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>93.49</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>98.21</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>98.82</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>97.23</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>98.63</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>107.45</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>122.57</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>116.09</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>99.55</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>93.92</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>96.56</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>95.83</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>92.76</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>97.86</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>98.26</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>97.07</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>96.9</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>101.15</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>109.44</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>91.91</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>85.42</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>86.13</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>90.09</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>90.85</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>91.3</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>95.86</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>96.66</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>97.17</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>95.7</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>107.07</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>125.21</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>116.57</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>96.65</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>93.27</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>95.15</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>94.79</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>92.41</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>97.66</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>101.53</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>98.87</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>92.92</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>101.65</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>124.32</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>110.86</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>95.97</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>93.21</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>93.81</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>95.48</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>93.78</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>97.66</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>102.76</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>97.56</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>96.95</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>104.43</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>125.66</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>114.47</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>100.04</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>96.29</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>95.64</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>99.02</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>93.49</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>98.08</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>99.32</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>97.18</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>99.41</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>113.45</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>131.05000000000001</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>123.33</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>94.47</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>98.44</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>102.27</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>101.17</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>98.35</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>104.69</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>103.68</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>101.15</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>104.59</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>110.51</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>127.63</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>116.89</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>104.06</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>99.13</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>102.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-42BF-4A38-AFC2-01EB577238DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="529750880"/>
+        <c:axId val="529751360"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="529750880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="yyyy\-mm\-dd" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="529751360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="529751360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="60"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="529750880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>163511</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C038BC3F-CE6C-04F4-3CC2-C6F03E47392E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,7 +2935,7 @@
   <dimension ref="A1:M286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12063,5 +14596,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GDP graph, new quarter function
</commit_message>
<xml_diff>
--- a/Data/data_NSA/Varmonth.xlsx
+++ b/Data/data_NSA/Varmonth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad5e0ae908eb1af8/Documentos/GitHub/gdp-forecasting-with-ML/Data/data_NSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_AD4D361C20488DEA4E38A0E30418638E5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDC03B5E-40F4-4A53-A604-738FB4DEA417}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_AD4D361C20488DEA4E38A0E30418638E5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CA3B874-726B-4489-BACB-4FF8A229939F}"/>
   <bookViews>
-    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="8805" yWindow="-9720" windowWidth="14400" windowHeight="7275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -2632,16 +2632,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>163511</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>3174</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2667,6 +2667,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2935,7 +2939,7 @@
   <dimension ref="A1:M286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>